<commit_message>
feat: basic simulated annealing works
</commit_message>
<xml_diff>
--- a/profillängen.xlsx
+++ b/profillängen.xlsx
@@ -104,31 +104,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -170,10 +167,60 @@
         <v>500</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>4570</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
feat: export of results to yaml files
</commit_message>
<xml_diff>
--- a/profillängen.xlsx
+++ b/profillängen.xlsx
@@ -97,8 +97,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -122,100 +126,80 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>4000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>800</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>2100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>700</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>300</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>240</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>520</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>670</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>100</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>1000</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>2000</v>
-      </c>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>2350</v>
-      </c>
+      <c r="A16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>4500</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>4570</v>
-      </c>
+      <c r="A18" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>